<commit_message>
Changed All Tests to Read from Excel Sheet
</commit_message>
<xml_diff>
--- a/src/test/resources/TestData.xlsx
+++ b/src/test/resources/TestData.xlsx
@@ -5,14 +5,16 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\yzakareya\healthi-test-automation\Data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\yzakareya\healthi-test-automation\src\test\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="14380" windowHeight="4190"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="LoginTest" sheetId="1" r:id="rId1"/>
+    <sheet name="NewMedicineService" sheetId="2" r:id="rId2"/>
+    <sheet name="PatientRecords" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -24,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="24">
   <si>
     <t>NewScreen</t>
   </si>
@@ -54,6 +56,48 @@
   </si>
   <si>
     <t>https://healthi-test.cegedim.com/pharmacy/Dashboard</t>
+  </si>
+  <si>
+    <t>ProductSearch</t>
+  </si>
+  <si>
+    <t>inProgressClinicalServicesExpected</t>
+  </si>
+  <si>
+    <t>InterventionDate</t>
+  </si>
+  <si>
+    <t>FollowUpDate</t>
+  </si>
+  <si>
+    <t>deliveredClinicalServicesExpected</t>
+  </si>
+  <si>
+    <t>Warfarin</t>
+  </si>
+  <si>
+    <t>13/01/2021</t>
+  </si>
+  <si>
+    <t>30</t>
+  </si>
+  <si>
+    <t>NewMedicine1</t>
+  </si>
+  <si>
+    <t>Surname</t>
+  </si>
+  <si>
+    <t>FirstName</t>
+  </si>
+  <si>
+    <t>PatientSearch1</t>
+  </si>
+  <si>
+    <t>Smith</t>
+  </si>
+  <si>
+    <t>Robert</t>
   </si>
 </sst>
 </file>
@@ -106,10 +150,12 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -394,7 +440,7 @@
   <dimension ref="A1:E2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B15" sqref="B15"/>
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -448,4 +494,112 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:F2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D18" sqref="D18"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="16.453125" style="4" customWidth="1"/>
+    <col min="2" max="2" width="16" style="4" customWidth="1"/>
+    <col min="3" max="3" width="31.1796875" style="4" customWidth="1"/>
+    <col min="4" max="4" width="17.08984375" style="4" customWidth="1"/>
+    <col min="5" max="5" width="17.7265625" style="4" customWidth="1"/>
+    <col min="6" max="6" width="30.81640625" style="4" customWidth="1"/>
+    <col min="7" max="16384" width="8.7265625" style="4"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A1" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="F1" s="3" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A2" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="B2" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="C2" s="4">
+        <v>36</v>
+      </c>
+      <c r="D2" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="E2" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="F2" s="4" t="s">
+        <v>17</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:C2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C1" sqref="C1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="15.26953125" customWidth="1"/>
+    <col min="2" max="2" width="13.6328125" customWidth="1"/>
+    <col min="3" max="3" width="14.54296875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A1" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
+        <v>21</v>
+      </c>
+      <c r="B2" t="s">
+        <v>22</v>
+      </c>
+      <c r="C2" t="s">
+        <v>23</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Changed All Tests to Read from Excel Sheet final
</commit_message>
<xml_diff>
--- a/src/test/resources/TestData.xlsx
+++ b/src/test/resources/TestData.xlsx
@@ -9,12 +9,13 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="14380" windowHeight="4190"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="14380" windowHeight="4190" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="LoginTest" sheetId="1" r:id="rId1"/>
-    <sheet name="NewMedicineService" sheetId="2" r:id="rId2"/>
-    <sheet name="PatientRecords" sheetId="3" r:id="rId3"/>
+    <sheet name="NHSFLuVaccService" sheetId="4" r:id="rId2"/>
+    <sheet name="NewMedicineService" sheetId="2" r:id="rId3"/>
+    <sheet name="PatientRecords" sheetId="3" r:id="rId4"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -26,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="35">
   <si>
     <t>NewScreen</t>
   </si>
@@ -98,6 +99,39 @@
   </si>
   <si>
     <t>Robert</t>
+  </si>
+  <si>
+    <t>DateOfAdmin</t>
+  </si>
+  <si>
+    <t>BatchNum</t>
+  </si>
+  <si>
+    <t>TimeOfAdmin</t>
+  </si>
+  <si>
+    <t>VaccineSearch</t>
+  </si>
+  <si>
+    <t>ExpiryDate</t>
+  </si>
+  <si>
+    <t>NHSFluVac1</t>
+  </si>
+  <si>
+    <t>21/01/2021</t>
+  </si>
+  <si>
+    <t>01:30 PM</t>
+  </si>
+  <si>
+    <t>GSK - Fluarix TM Tetra (pack size 10)</t>
+  </si>
+  <si>
+    <t>12345</t>
+  </si>
+  <si>
+    <t>01/2021</t>
   </si>
 </sst>
 </file>
@@ -439,7 +473,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
@@ -497,6 +531,71 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:F2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E17" sqref="E17"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="16.08984375" style="4" customWidth="1"/>
+    <col min="2" max="2" width="13.1796875" style="4" customWidth="1"/>
+    <col min="3" max="3" width="14.08984375" style="4" customWidth="1"/>
+    <col min="4" max="4" width="33.81640625" style="4" customWidth="1"/>
+    <col min="5" max="5" width="11.453125" style="4" customWidth="1"/>
+    <col min="6" max="6" width="10.7265625" style="4" customWidth="1"/>
+    <col min="7" max="16384" width="8.7265625" style="4"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A1" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="F1" s="3" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A2" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="B2" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="C2" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="D2" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="E2" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="F2" s="4" t="s">
+        <v>34</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F2"/>
   <sheetViews>
@@ -561,7 +660,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C2"/>
   <sheetViews>

</xml_diff>